<commit_message>
Implement ISO, UPPER_CASE and male/female
</commit_message>
<xml_diff>
--- a/injury_data.xlsx
+++ b/injury_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,237 +441,520 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>SEX</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Team</t>
+          <t>NAME</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Code</t>
+          <t>TEAM</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Injury Date</t>
+          <t>CODE</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Return Date</t>
+          <t>INJURY_DATE</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Injury Location</t>
+          <t>RETURN_DATE</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Injury Side</t>
+          <t>INJURY_LOCATION</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Injury Type</t>
+          <t>INJURY_SIDE</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Occurrence</t>
+          <t>INJURY_TYPE</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Overuse/Trauma</t>
+          <t>OCCURRENCE</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Onset</t>
+          <t>OVERUSE_TRAUMA</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>ONSET</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>CONTACT</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Action Description</t>
+          <t>ACTION</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Re-injury</t>
+          <t>ACTION_DESCRIPTION</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Referee Sanction</t>
+          <t>RE_INJURY</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Diagnostic Examination</t>
+          <t>REFEREE_SANCTION</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Diagnosis</t>
+          <t>DIAGNOSTIC_EXAMINATION</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Surgery</t>
+          <t>DIAGNOSIS</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Menstrual Phase</t>
+          <t>SURGERY</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Oral Contraceptives</t>
+          <t>MENSTRUAL_PHASE</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Hormonal Contraceptives</t>
+          <t>ORAL_CONTRACEPTIVES</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Other Comments</t>
+          <t>HORMONAL_CONTRACEPTIVES</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>OTHER_COMMENTS</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>1.docx</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2.docx</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Luca F</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>FC B</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>xx11x</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-06-23</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Wrong date format</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Lower leg (incl. Achilles tendon)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Bilateral/central</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Muscle rupture/tear/strain**</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>N/A (gradual onset injury)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Overuse (repetitive mechanism)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Gradual onset</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>No foul, Opponent foul, Own foul, Yellow card, Red card</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Ultrasonography</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Should appear</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3.docx</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>All filled</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>FC ALL</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>XXXXX</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-10-12</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Head, Abdomen, Elbow, Hip, Lower leg (incl. Achilles tendon), Neck, Lumbosacral, Forearm, Groin, Ankle, Chest, Shoulder, Wrist, Thigh, Foot, Thoracic spine, Upper arm, Hand, Knee</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Right, Left, Bilateral/central</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Concussion, Meniscus lesion, Haematoma/contusion/bruise (incl. compartment syndrome), Fracture (specify if stress fracture), Cartilage lesion, Nerve injury (central or peripheral other than concussion), Other bone injury (e.g., bone stress), Muscle rupture/tear/strain**, Dental injury*, Joint dislocation/subluxation*, Tendon rupture/tendinopathy, Vessel injury (excl. skin haematoma), Joint sprain (i.e., ligament/capsule), Abrasion, Bursitis, Arthritis/synovitis/capsulitis, Laceration, Overuse unspecified, Additional Injury</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Training, Match (min. of injury: 70), N/A (gradual onset injury), Football training, Football &amp; other training, League match, Friendly match, Other training, Reserve/youth team training, Champions League, Reserve/youth team match, National team, Other cup match</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Running/sprinting, Heading, Controlling the ball, Tackling other player, Blocked*, Twisting/turning, Landing (incl. jumping), Hit by ball, Tackled by other player, Use of arm/elbow*, Shooting/passing, Falling (incl. diving), Collision, Sliding/stretching*, Other player action</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Did everything</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>No foul, Opponent foul, Own foul, Yellow card, Red card</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Clinical only, X-ray, Ultrasonography, MRI, Other</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>DIagnosis</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>xxxx_yy.docx</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>NAME SURNAME</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>TEAM_NAME</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>TEAM:CODE</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2022-5-3</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2022-6-3</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2022-05-03</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2022-06-03</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>Thigh</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Left</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>Joint sprain (i.e., ligament/capsule)</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>Match (min. of injury: 70), National team</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>Trauma (acute mechanism)</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>Sudden onset</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Yes, direct contact (to injured body part)</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>Falling (incl. diving)</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>direct contact to the A-C joint on an unprotected fall</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>Opponent foul</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>MRI</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>A-C joint II degree sprain</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="W5" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="X5" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Swap map fix for old files
</commit_message>
<xml_diff>
--- a/injury_data.xlsx
+++ b/injury_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,117 +446,142 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>FILE_FORMAT</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>NAME</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>TEAM</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>CODE</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>INJURY_DATE</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>RETURN_DATE</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>INJURY_LOCATION</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>INJURY_SIDE</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>INJURY_TYPE</t>
-        </is>
-      </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>OCCURRENCE</t>
+          <t>TYPE</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>OCCURRENCE_ONSET_TYPE</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>OCCURRENCE_MATCH_MINUTE</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>OCCURRENCE_CONTEXT</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>OVERUSE_TRAUMA</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>ONSET</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>CONTACT</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>ACTION</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>ACTION_DESCRIPTION</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>RE_INJURY</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>RECURRENCE</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>PREVIOUS_RETURN_DATE</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>REFEREE_SANCTION</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>DIAGNOSTIC_EXAMINATION</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>DIAGNOSIS</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>SURGERY</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>MENSTRUAL_PHASE</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>ORAL_CONTRACEPTIVES</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>HORMONAL_CONTRACEPTIVES</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>OTHER_COMMENTS</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>UPDATED_AT</t>
         </is>
       </c>
     </row>
@@ -573,101 +598,122 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Neymar</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>PSG</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>xx11asx</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>2024-06-23</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>2025-05-18</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
         <is>
           <t>Right, Left, Bilateral/central</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Muscle rupture/tear/strain**, Other injury</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Match, Friendly match</t>
-        </is>
-      </c>
       <c r="L2" t="inlineStr">
         <is>
+          <t>Match</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Friendly match</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
           <t>Both, Overuse and Trauma</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>Sudden onset</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>Yes, direct contact (to injured body part)</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr">
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr">
         <is>
           <t>Dive</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr">
         <is>
           <t>No foul, Opponent foul, Own foul, Yellow card, Red card</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr">
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
         <is>
           <t>No comment</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:51</t>
         </is>
       </c>
     </row>
@@ -684,101 +730,122 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Neymar</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>PSG</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>xx11asx</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>2024-06-23</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>2025-05-18</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
         <is>
           <t>Right, Left, Bilateral/central</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>Muscle rupture/tear/strain**, Other injury</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Match, Friendly match</t>
-        </is>
-      </c>
       <c r="L3" t="inlineStr">
         <is>
+          <t>Match</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Friendly match</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
           <t>Both, Overuse and Trauma</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>Sudden onset</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Yes, direct contact (to injured body part)</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr">
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr">
         <is>
           <t>Dive</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr">
         <is>
           <t>No foul, Opponent foul, Own foul, Yellow card, Red card</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Ultrasonography</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr">
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
         <is>
           <t>No comment</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:51</t>
         </is>
       </c>
     </row>
@@ -793,7 +860,11 @@
           <t>Male</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>OLD</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -816,6 +887,15 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:51</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -828,7 +908,11 @@
           <t>Male</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>OLD</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
@@ -851,6 +935,15 @@
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:52</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -865,101 +958,114 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>Luca F</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>FC B</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>xx11x</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>2025-06-23</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Wrong date format</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Lower leg (incl. Achilles tendon), Thigh</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>Left, Bilateral/central</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>Muscle rupture/tear/strain**</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
         <is>
           <t>Friendly match</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>Overuse (repetitive mechanism)</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>Both, Gradual and Sudden</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>Yes, direct contact (to injured body part)</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr">
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr">
         <is>
           <t>Twisted the knee</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr">
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr">
         <is>
           <t>No foul, Opponent foul, Own foul, Yellow card, Red card</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="W6" t="inlineStr">
         <is>
           <t>Ultrasonography</t>
         </is>
       </c>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr">
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr">
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
         <is>
           <t>No comment</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:52</t>
         </is>
       </c>
     </row>
@@ -976,101 +1082,114 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>Luca F</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>FC B</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>xx11x</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>2025-06-23</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>Wrong date format</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Lower leg (incl. Achilles tendon), Thigh</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>Left, Bilateral/central</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>Muscle rupture/tear/strain**</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
         <is>
           <t>Friendly match</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>Overuse (repetitive mechanism)</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>Both, Gradual and Sudden</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>Yes, direct contact (to injured body part)</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr">
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr">
         <is>
           <t>Twisted the knee</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr">
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr">
         <is>
           <t>No foul, Opponent foul, Own foul, Yellow card, Red card</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>X-ray</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr">
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>Ultrasonography</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr">
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
         <is>
           <t>No comment</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:52</t>
         </is>
       </c>
     </row>
@@ -1087,117 +1206,138 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>All filled</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>FC ALL</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>XXXXX</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>2025-06-10</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>2025-10-12</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Head, Abdomen, Elbow, Hip, Lower leg (incl. Achilles tendon), Neck, Lumbosacral, Forearm, Groin, Ankle, Chest, Shoulder, Wrist, Thigh, Foot, Thoracic spine, Upper arm, Hand, Knee</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>Right, Left, Bilateral/central</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>Concussion, Meniscus lesion, Haematoma/contusion/bruise (incl. compartment syndrome), Fracture (specify if stress fracture), Cartilage lesion, Nerve injury (central or peripheral other than concussion), Other bone injury (e.g., bone stress), Muscle rupture/tear/strain**, Dental injury*, Joint dislocation/subluxation*, Tendon rupture/tendinopathy, Vessel injury (excl. skin haematoma), Joint sprain (i.e., ligament/capsule), Abrasion, Bursitis, Arthritis/synovitis/capsulitis, Laceration, Overuse unspecified, Additional Injury</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Training, Match (min. of injury: 70), N/A (gradual onset injury), Football training, Football &amp; other training, League match, Friendly match, Other training, Reserve/youth team training, Champions League, Reserve/youth team match, National team, Other cup match</t>
-        </is>
-      </c>
       <c r="L8" t="inlineStr">
         <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Football training, Football &amp; other training, League match, Friendly match, Other training, Reserve/youth team training, Champions League, Reserve/youth team match, National team, Other cup match</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
           <t>Both, Overuse and Trauma</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>Both, Gradual and Sudden</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
         <is>
           <t>Running/sprinting, Heading, Controlling the ball, Tackling other player, Blocked*, Twisting/turning, Landing (incl. jumping), Hit by ball, Tackled by other player, Use of arm/elbow*, Shooting/passing, Falling (incl. diving), Collision, Sliding/stretching*, Other player action</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>Did everything</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr">
         <is>
           <t>No foul, Opponent foul, Own foul, Yellow card, Red card</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="W8" t="inlineStr">
         <is>
           <t>Clinical only, X-ray, Ultrasonography, MRI, Other</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="X8" t="inlineStr">
         <is>
           <t>DIagnosis</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
       <c r="Y8" t="inlineStr">
         <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
           <t>Comment</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:53</t>
         </is>
       </c>
     </row>
@@ -1214,117 +1354,134 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>All filled</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>FC ALL</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>XXXXX</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>2025-06-10</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>2025-10-12</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>Head, Abdomen, Elbow, Hip, Lower leg (incl. Achilles tendon), Neck, Lumbosacral, Forearm, Groin, Ankle, Chest, Shoulder, Wrist, Thigh, Foot, Thoracic spine, Upper arm, Hand, Knee</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>Right, Left, Bilateral/central</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>Concussion, Meniscus lesion, Haematoma/contusion/bruise (incl. compartment syndrome), Fracture (specify if stress fracture), Cartilage lesion, Nerve injury (central or peripheral other than concussion), Other bone injury (e.g., bone stress), Muscle rupture/tear/strain**, Dental injury*, Joint dislocation/subluxation*, Tendon rupture/tendinopathy, Vessel injury (excl. skin haematoma), Joint sprain (i.e., ligament/capsule), Abrasion, Bursitis, Arthritis/synovitis/capsulitis, Laceration, Overuse unspecified, Additional Injury</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Training, Match (min. of injury: 70), N/A (gradual onset injury), Football training, Football &amp; other training, League match, Friendly match, Other training, Reserve/youth team training, Champions League, Reserve/youth team match, National team, Other cup match</t>
-        </is>
-      </c>
       <c r="L9" t="inlineStr">
         <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Football training, Football &amp; other training, League match, Friendly match, Other training, Reserve/youth team training, Champions League, Reserve/youth team match, National team, Other cup match</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
           <t>Both, Overuse and Trauma</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>Both, Gradual and Sudden</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
         <is>
           <t>Running/sprinting, Heading, Controlling the ball, Tackling other player, Blocked*, Twisting/turning, Landing (incl. jumping), Hit by ball, Tackled by other player, Use of arm/elbow*, Shooting/passing, Falling (incl. diving), Collision, Sliding/stretching*, Other player action</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>Did everything</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr">
         <is>
           <t>No foul, Opponent foul, Own foul, Yellow card, Red card</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="W9" t="inlineStr">
         <is>
           <t>Clinical only, X-ray, Ultrasonography, MRI, Other</t>
         </is>
       </c>
-      <c r="T9" t="inlineStr">
+      <c r="X9" t="inlineStr">
         <is>
           <t>DIagnosis</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
       <c r="Y9" t="inlineStr">
         <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
           <t>Comment</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:53</t>
         </is>
       </c>
     </row>
@@ -1341,117 +1498,134 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>All filled</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>FC ALL</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>XXXXX</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>2025-06-10</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>2025-10-12</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Head, Abdomen, Elbow, Hip, Lower leg (incl. Achilles tendon), Neck, Lumbosacral, Forearm, Groin, Ankle, Chest, Shoulder, Wrist, Thigh, Foot, Thoracic spine, Upper arm, Hand, Knee</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>Right, Left, Bilateral/central</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>Concussion, Meniscus lesion, Haematoma/contusion/bruise (incl. compartment syndrome), Fracture (specify if stress fracture), Cartilage lesion, Nerve injury (central or peripheral other than concussion), Other bone injury (e.g., bone stress), Muscle rupture/tear/strain**, Dental injury*, Joint dislocation/subluxation*, Tendon rupture/tendinopathy, Vessel injury (excl. skin haematoma), Joint sprain (i.e., ligament/capsule), Abrasion, Bursitis, Arthritis/synovitis/capsulitis, Laceration, Overuse unspecified, Additional Injury</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Training, Match (min. of injury: 70), N/A (gradual onset injury), Football training, Football &amp; other training, League match, Friendly match, Other training, Reserve/youth team training, Champions League, Reserve/youth team match, National team, Other cup match</t>
-        </is>
-      </c>
       <c r="L10" t="inlineStr">
         <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Football training, Football &amp; other training, League match, Friendly match, Other training, Reserve/youth team training, Champions League, Reserve/youth team match, National team, Other cup match</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
           <t>Both, Overuse and Trauma</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>Both, Gradual and Sudden</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
         <is>
           <t>Running/sprinting, Heading, Controlling the ball, Tackling other player, Blocked*, Twisting/turning, Landing (incl. jumping), Hit by ball, Tackled by other player, Use of arm/elbow*, Shooting/passing, Falling (incl. diving), Collision, Sliding/stretching*, Other player action</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="S10" t="inlineStr">
         <is>
           <t>Did everything</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr">
         <is>
           <t>No foul, Opponent foul, Own foul, Yellow card, Red card</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="W10" t="inlineStr">
         <is>
           <t>Clinical only, X-ray, Ultrasonography, MRI, Other</t>
         </is>
       </c>
-      <c r="T10" t="inlineStr">
+      <c r="X10" t="inlineStr">
         <is>
           <t>DIagnosis</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>Too many answers</t>
-        </is>
-      </c>
       <c r="Y10" t="inlineStr">
         <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>Too many answers</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
           <t>Comment</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:54</t>
         </is>
       </c>
     </row>
@@ -1468,115 +1642,136 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>NAME SURNAME</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>TEAM_NAME</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>TEAM:CODE</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>2022-05-03</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>2022-06-03</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Thigh</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>Left</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>Custom Injury</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Match (min. of injury: 70), National team</t>
-        </is>
-      </c>
       <c r="L11" t="inlineStr">
         <is>
+          <t>Match</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>National team</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
           <t>Trauma (acute mechanism)</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>Sudden onset</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>Yes, direct contact (to injured body part)</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="R11" t="inlineStr">
         <is>
           <t>Falling (incl. diving)</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="S11" t="inlineStr">
         <is>
           <t>direct contact to the A-C joint on an unprotected fall</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>Yes, 08.06.2014</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr">
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr">
         <is>
           <t>Opponent foul</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="W11" t="inlineStr">
         <is>
           <t>MRI, Custom Exam</t>
         </is>
       </c>
-      <c r="T11" t="inlineStr">
+      <c r="X11" t="inlineStr">
         <is>
           <t>A-C joint II degree sprain</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr">
+      <c r="Y11" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="V11" t="inlineStr">
+      <c r="Z11" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="W11" t="inlineStr">
+      <c r="AA11" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="X11" t="inlineStr">
+      <c r="AB11" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="Y11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:54</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1591,115 +1786,136 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>NAME SURNAME</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>TEAM_NAME</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>TEAM:CODE</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>2022-05-03</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>2022-06-03</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Thigh</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>Left</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>Custom Injury</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Match (min. of injury: 70), Other cup match</t>
-        </is>
-      </c>
       <c r="L12" t="inlineStr">
         <is>
+          <t>Match</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>National team</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
           <t>Trauma (acute mechanism)</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>Sudden onset</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>Yes, direct contact (to injured body part)</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="R12" t="inlineStr">
         <is>
           <t>Falling (incl. diving)</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="S12" t="inlineStr">
         <is>
           <t>direct contact to the A-C joint on an unprotected fall</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>Yes, 08.06.2014</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>No foul</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>Ultrasonography, Custom Exam</t>
-        </is>
-      </c>
-      <c r="T12" t="inlineStr">
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>Opponent foul</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>MRI, Custom Exam</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
         <is>
           <t>A-C joint II degree sprain</t>
         </is>
       </c>
-      <c r="U12" t="inlineStr">
+      <c r="Y12" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="V12" t="inlineStr">
+      <c r="Z12" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="W12" t="inlineStr">
+      <c r="AA12" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="X12" t="inlineStr">
+      <c r="AB12" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="Y12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:54</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1714,115 +1930,136 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>NAME SURNAME</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>TEAM_NAME</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>TEAM:CODE</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>2022-05-03</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>2022-06-03</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>Thigh</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>Left</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>Joint sprain (i.e., ligament/capsule)</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Match (min. of injury: 70), National team</t>
-        </is>
-      </c>
       <c r="L13" t="inlineStr">
         <is>
+          <t>Match</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>National team</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
           <t>Trauma (acute mechanism)</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>Sudden onset</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>Yes, direct contact (to injured body part)</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="R13" t="inlineStr">
         <is>
           <t>Falling (incl. diving)</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="S13" t="inlineStr">
         <is>
           <t>direct contact to the A-C joint on an unprotected fall</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
+      <c r="T13" t="inlineStr">
         <is>
           <t>Yes, random text</t>
         </is>
       </c>
-      <c r="R13" t="inlineStr">
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr">
         <is>
           <t>Opponent foul</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr">
+      <c r="W13" t="inlineStr">
         <is>
           <t>MRI</t>
         </is>
       </c>
-      <c r="T13" t="inlineStr">
+      <c r="X13" t="inlineStr">
         <is>
           <t>A-C joint II degree sprain</t>
         </is>
       </c>
-      <c r="U13" t="inlineStr">
+      <c r="Y13" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="V13" t="inlineStr">
+      <c r="Z13" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="W13" t="inlineStr">
+      <c r="AA13" t="inlineStr">
         <is>
           <t>Yes, Using Contra 1</t>
         </is>
       </c>
-      <c r="X13" t="inlineStr">
+      <c r="AB13" t="inlineStr">
         <is>
           <t>Yes, Using Hormone 1</t>
         </is>
       </c>
-      <c r="Y13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:54</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1837,115 +2074,136 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>NAME SURNAME</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>TEAM_NAME</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>TEAM:CODE</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>2022-05-03</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>2022-06-03</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Thigh</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>Left</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>Joint sprain (i.e., ligament/capsule)</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Match (min. of injury: 70), Other cup match</t>
-        </is>
-      </c>
       <c r="L14" t="inlineStr">
         <is>
+          <t>Match</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>National team</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
           <t>Trauma (acute mechanism)</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>Sudden onset</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>Yes, direct contact (to injured body part)</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="R14" t="inlineStr">
         <is>
           <t>Falling (incl. diving)</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="S14" t="inlineStr">
         <is>
           <t>direct contact to the A-C joint on an unprotected fall</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
+      <c r="T14" t="inlineStr">
         <is>
           <t>Yes, random text</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>No foul</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>Opponent foul</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>MRI</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
         <is>
           <t>A-C joint II degree sprain</t>
         </is>
       </c>
-      <c r="U14" t="inlineStr">
+      <c r="Y14" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="V14" t="inlineStr">
+      <c r="Z14" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="W14" t="inlineStr">
+      <c r="AA14" t="inlineStr">
         <is>
           <t>Yes, Using Contra 1</t>
         </is>
       </c>
-      <c r="X14" t="inlineStr">
+      <c r="AB14" t="inlineStr">
         <is>
           <t>Yes, Using Hormone 1</t>
         </is>
       </c>
-      <c r="Y14" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:55</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1960,115 +2218,136 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>NAME SURNAME</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>TEAM_NAME</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>TEAM:CODE</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>2022-05-03</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>2022-06-03</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>Thigh</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>Left</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>Joint sprain (i.e., ligament/capsule)</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>Match (min. of injury: 70), National team</t>
-        </is>
-      </c>
       <c r="L15" t="inlineStr">
         <is>
+          <t>Match</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>National team</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
           <t>Trauma (acute mechanism)</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>Sudden onset</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>Yes, direct contact (to injured body part)</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="R15" t="inlineStr">
         <is>
           <t>Falling (incl. diving)</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="S15" t="inlineStr">
         <is>
           <t>direct contact to the A-C joint on an unprotected fall</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
+      <c r="T15" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr">
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr">
         <is>
           <t>Opponent foul</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr">
+      <c r="W15" t="inlineStr">
         <is>
           <t>MRI</t>
         </is>
       </c>
-      <c r="T15" t="inlineStr">
+      <c r="X15" t="inlineStr">
         <is>
           <t>A-C joint II degree sprain</t>
         </is>
       </c>
-      <c r="U15" t="inlineStr">
+      <c r="Y15" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="V15" t="inlineStr">
+      <c r="Z15" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="W15" t="inlineStr">
+      <c r="AA15" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="X15" t="inlineStr">
+      <c r="AB15" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="Y15" t="inlineStr"/>
+      <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:55</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2083,115 +2362,136 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>OLD</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>NAME SURNAME</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>TEAM_NAME</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>TEAM:CODE</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>2022-05-03</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>2022-06-03</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>Thigh</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>Left</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>Joint sprain (i.e., ligament/capsule)</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>Match (min. of injury: 70), Other cup match</t>
-        </is>
-      </c>
       <c r="L16" t="inlineStr">
         <is>
+          <t>Match</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>National team</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
           <t>Trauma (acute mechanism)</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>Sudden onset</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
+      <c r="Q16" t="inlineStr">
         <is>
           <t>Yes, direct contact (to injured body part)</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="R16" t="inlineStr">
         <is>
           <t>Falling (incl. diving)</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="S16" t="inlineStr">
         <is>
           <t>direct contact to the A-C joint on an unprotected fall</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>No foul</t>
-        </is>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
       <c r="T16" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>Opponent foul</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>MRI</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
           <t>A-C joint II degree sprain</t>
         </is>
       </c>
-      <c r="U16" t="inlineStr">
+      <c r="Y16" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="V16" t="inlineStr">
+      <c r="Z16" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="W16" t="inlineStr">
+      <c r="AA16" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="X16" t="inlineStr">
+      <c r="AB16" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="Y16" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>2025-11-10 13:02:55</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>